<commit_message>
cambios antes de gemini cmpt
</commit_message>
<xml_diff>
--- a/tableros/tableros_gal_ES.xlsx
+++ b/tableros/tableros_gal_ES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\OneDrive - Universidade da Coruña\UDC4\TFG\ComunicELA-tfg\tableros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579D8E6D-584E-4891-A6BC-02EF0122CCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E3F5B2-01C8-4097-BCF6-A1F8B6F297BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inicial" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>CARNE</t>
   </si>
   <si>
-    <t>PESCADO</t>
-  </si>
-  <si>
     <t>PIZZA</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>PAN</t>
   </si>
   <si>
-    <t>SANDWICH</t>
-  </si>
-  <si>
     <t>GALLETAS</t>
   </si>
   <si>
@@ -184,9 +178,6 @@
     <t>BAÑO</t>
   </si>
   <si>
-    <t>PASILLO</t>
-  </si>
-  <si>
     <t>ASCENSOR</t>
   </si>
   <si>
@@ -217,9 +208,6 @@
     <t>ANTES</t>
   </si>
   <si>
-    <t>AHORA</t>
-  </si>
-  <si>
     <t>DENTRO</t>
   </si>
   <si>
@@ -241,9 +229,6 @@
     <t>PURÉ</t>
   </si>
   <si>
-    <t>JAMÓN</t>
-  </si>
-  <si>
     <t>BATERÍA</t>
   </si>
   <si>
@@ -265,9 +250,6 @@
     <t>SOFÁ</t>
   </si>
   <si>
-    <t>DELFÍN</t>
-  </si>
-  <si>
     <t>SÍ</t>
   </si>
   <si>
@@ -784,9 +766,6 @@
     <t>FABAS</t>
   </si>
   <si>
-    <t>PITO</t>
-  </si>
-  <si>
     <t>LENTELLAS</t>
   </si>
   <si>
@@ -814,9 +793,6 @@
     <t>PARAUGAS</t>
   </si>
   <si>
-    <t>LENTES</t>
-  </si>
-  <si>
     <t>RELOXO</t>
   </si>
   <si>
@@ -826,18 +802,6 @@
     <t>PAI</t>
   </si>
   <si>
-    <t>NÓS-AS</t>
-  </si>
-  <si>
-    <t>EL-ELA</t>
-  </si>
-  <si>
-    <t>ELES-ELAS</t>
-  </si>
-  <si>
-    <t>VÓS-AS</t>
-  </si>
-  <si>
     <t>NAI</t>
   </si>
   <si>
@@ -932,6 +896,42 @@
   </si>
   <si>
     <t>FÓRA</t>
+  </si>
+  <si>
+    <t>PEIXE</t>
+  </si>
+  <si>
+    <t>POLO</t>
+  </si>
+  <si>
+    <t>SÁNDWICH</t>
+  </si>
+  <si>
+    <t>XAMÓN</t>
+  </si>
+  <si>
+    <t>ANTEOLLOS</t>
+  </si>
+  <si>
+    <t>NÓS</t>
+  </si>
+  <si>
+    <t>VÓS</t>
+  </si>
+  <si>
+    <t>EL-A</t>
+  </si>
+  <si>
+    <t>ELES-AS</t>
+  </si>
+  <si>
+    <t>GOLFIÑO</t>
+  </si>
+  <si>
+    <t>AGORA</t>
+  </si>
+  <si>
+    <t>CORREDOR</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1267,51 +1267,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="H1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -1319,25 +1319,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E3" t="s">
         <v>218</v>
       </c>
-      <c r="B3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E3" t="s">
-        <v>224</v>
-      </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
@@ -1365,80 +1365,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" t="s">
-        <v>180</v>
-      </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
         <v>172</v>
       </c>
-      <c r="B2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
         <v>175</v>
       </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>181</v>
-      </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
         <v>173</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>176</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>43</v>
-      </c>
-      <c r="E3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1450,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50E60F1-2F1E-4687-9D5F-1A293A57DF1A}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1461,80 +1461,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F1" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="G1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="H1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" t="s">
         <v>183</v>
       </c>
-      <c r="B2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>189</v>
-      </c>
       <c r="F2" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="G2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H2" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E3" t="s">
         <v>184</v>
       </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E3" t="s">
-        <v>190</v>
-      </c>
       <c r="F3" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="G3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1547,7 +1547,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1560,80 +1560,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="E1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="H1" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F2" t="s">
+        <v>269</v>
+      </c>
+      <c r="G2" t="s">
         <v>196</v>
       </c>
-      <c r="D2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F2" t="s">
-        <v>281</v>
-      </c>
-      <c r="G2" t="s">
-        <v>202</v>
-      </c>
       <c r="H2" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G3" t="s">
         <v>197</v>
       </c>
-      <c r="D3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" t="s">
-        <v>200</v>
-      </c>
-      <c r="F3" t="s">
-        <v>280</v>
-      </c>
-      <c r="G3" t="s">
-        <v>203</v>
-      </c>
       <c r="H3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1656,80 +1656,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" t="s">
-        <v>285</v>
-      </c>
-      <c r="G1" t="s">
-        <v>89</v>
-      </c>
       <c r="H1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
         <v>84</v>
       </c>
-      <c r="D2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
-      </c>
       <c r="H2" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
         <v>85</v>
       </c>
-      <c r="D3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>91</v>
-      </c>
       <c r="H3" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -1741,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0BAF42D-658C-4F53-B46F-DDD16A5FEECB}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1753,80 +1753,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D1" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="E1" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="G1" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="H1" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>204</v>
       </c>
-      <c r="B2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>210</v>
-      </c>
       <c r="F2" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="G2" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E3" t="s">
         <v>205</v>
       </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D3" t="s">
-        <v>297</v>
-      </c>
-      <c r="E3" t="s">
-        <v>211</v>
-      </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="H3" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -1852,51 +1852,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E2" t="s">
         <v>94</v>
       </c>
-      <c r="B2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
         <v>97</v>
-      </c>
-      <c r="D2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" t="s">
-        <v>103</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -1904,25 +1904,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G3" t="s">
         <v>98</v>
-      </c>
-      <c r="D3" t="s">
-        <v>235</v>
-      </c>
-      <c r="E3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" t="s">
-        <v>238</v>
-      </c>
-      <c r="G3" t="s">
-        <v>104</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -1950,25 +1950,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1976,51 +1976,51 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -2049,51 +2049,51 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="G1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -2101,28 +2101,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2135,7 +2135,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2148,80 +2148,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H1" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H2" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>286</v>
       </c>
       <c r="G3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H3" t="s">
-        <v>248</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2234,7 +2234,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,80 +2247,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" t="s">
         <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G2" t="s">
         <v>134</v>
       </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G2" t="s">
-        <v>140</v>
-      </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" t="s">
         <v>135</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G3" t="s">
-        <v>141</v>
-      </c>
       <c r="H3" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2333,7 +2333,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2346,80 +2346,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" t="s">
         <v>144</v>
       </c>
-      <c r="D1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>150</v>
-      </c>
       <c r="H1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E2" t="s">
         <v>142</v>
       </c>
-      <c r="B2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G2" t="s">
         <v>145</v>
       </c>
-      <c r="D2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F2" t="s">
-        <v>259</v>
-      </c>
-      <c r="G2" t="s">
-        <v>151</v>
-      </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
         <v>143</v>
       </c>
-      <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
         <v>146</v>
       </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" t="s">
-        <v>152</v>
-      </c>
       <c r="H3" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2432,7 +2432,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2445,80 +2445,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
-        <v>262</v>
+        <v>291</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H1" t="s">
-        <v>263</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H2" t="s">
-        <v>264</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G3" t="s">
         <v>155</v>
       </c>
-      <c r="D3" t="s">
-        <v>261</v>
-      </c>
-      <c r="E3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F3" t="s">
-        <v>266</v>
-      </c>
-      <c r="G3" t="s">
-        <v>161</v>
-      </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2543,80 +2543,80 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F1" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="G1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
         <v>162</v>
       </c>
-      <c r="B2" t="s">
-        <v>268</v>
-      </c>
-      <c r="C2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>168</v>
-      </c>
       <c r="F2" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="G2" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H2" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
         <v>163</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>